<commit_message>
xlsx files updated; Reviews and Gon. Gomes work missing;
Signed-off-by: GoncaloRodri <gg.rodrigues@campus.fct.unl.pt>
</commit_message>
<xml_diff>
--- a/project/Phase1/Sprint1/Burndown Chart.xlsx
+++ b/project/Phase1/Sprint1/Burndown Chart.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Sprint 1 Burndown Chart</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Ideal Burndown</t>
-  </si>
-  <si>
-    <t>15  = 3 cada</t>
   </si>
 </sst>
 </file>
@@ -465,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -511,9 +508,6 @@
     <xf borderId="5" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="11" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -528,9 +522,6 @@
     </xf>
     <xf borderId="12" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf borderId="15" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
@@ -648,8 +639,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1604795113"/>
-        <c:axId val="1096823797"/>
+        <c:axId val="2028821205"/>
+        <c:axId val="2076403543"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -723,11 +714,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1604795113"/>
-        <c:axId val="1096823797"/>
+        <c:axId val="2028821205"/>
+        <c:axId val="2076403543"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1604795113"/>
+        <c:axId val="2028821205"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -779,10 +770,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1096823797"/>
+        <c:crossAx val="2076403543"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1096823797"/>
+        <c:axId val="2076403543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30.0"/>
@@ -847,7 +838,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1604795113"/>
+        <c:crossAx val="2028821205"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1267,206 +1258,210 @@
       <c r="L6" s="16">
         <v>4.0</v>
       </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
+      <c r="M6" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
     </row>
     <row r="7">
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <v>2.0</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="19">
         <v>10.0</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="20">
         <v>0.0</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="21">
         <v>0.0</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="21">
         <v>0.0</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="21">
         <v>0.0</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="21">
         <v>0.0</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="21">
         <v>0.0</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="21">
         <v>0.0</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="21">
         <v>4.0</v>
       </c>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
+      <c r="M7" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
     </row>
     <row r="8">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26">
+      <c r="C8" s="23"/>
+      <c r="D8" s="24">
         <v>0.0</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <f t="shared" ref="E8:O8" si="1">SUM(E6:E7)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="27">
+      <c r="K8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L8" s="27">
+      <c r="L8" s="25">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="M8" s="27">
+      <c r="M8" s="25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="N8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N8" s="27">
+      <c r="O8" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="28"/>
+      <c r="P8" s="26"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31">
+      <c r="C9" s="28"/>
+      <c r="D9" s="29">
         <f>SUM(D6:D8)</f>
         <v>25</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="30">
         <f t="shared" ref="E9:O9" si="2">D9-SUM(E6:E7)</f>
         <v>25</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="31">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="31">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="31">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="31">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="32">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9" s="32">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="L9" s="34">
+      <c r="L9" s="32">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="M9" s="34">
+      <c r="M9" s="32">
         <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="N9" s="33">
+        <v>13</v>
+      </c>
+      <c r="N9" s="31">
         <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="O9" s="34">
+        <v>13</v>
+      </c>
+      <c r="O9" s="32">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="37">
+      <c r="C10" s="34"/>
+      <c r="D10" s="35">
         <f>D9</f>
         <v>25</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="36">
         <f>$D$10-($D$10/11*1)</f>
         <v>22.72727273</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="37">
         <f>$D$10-($D$10/11*2)</f>
         <v>20.45454545</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="37">
         <f>$D$10-($D$10/11*3)</f>
         <v>18.18181818</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="37">
         <f>$D$10-($D$10/11*4)</f>
         <v>15.90909091</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="37">
         <f>$D$10-($D$10/11*5)</f>
         <v>13.63636364</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="37">
         <f>$D$10-($D$10/11*6)</f>
         <v>11.36363636</v>
       </c>
-      <c r="K10" s="39">
+      <c r="K10" s="37">
         <f>$D$10-($D$10/11*7)</f>
         <v>9.090909091</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10" s="37">
         <f>$D$10-($D$10/11*8)</f>
         <v>6.818181818</v>
       </c>
-      <c r="M10" s="39">
+      <c r="M10" s="37">
         <f>$D$10-($D$10/11*9)</f>
         <v>4.545454545</v>
       </c>
-      <c r="N10" s="39">
+      <c r="N10" s="37">
         <f>$D$10-($D$10/11*10)</f>
         <v>2.272727273</v>
       </c>
-      <c r="O10" s="39">
+      <c r="O10" s="37">
         <f>$D$10-($D$10/11*11)</f>
         <v>0</v>
       </c>
@@ -1476,15 +1471,11 @@
     <row r="13" ht="15.75" customHeight="1"/>
     <row r="14" ht="15.75" customHeight="1"/>
     <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="L16" s="40" t="s">
-        <v>21</v>
-      </c>
-    </row>
+    <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="D19" s="40">
+      <c r="D19" s="38">
         <v>5.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ScrumMaster:Updated  burndownchart & sprintbacklog
Signed-off-by: GoncaloRodri <gg.rodrigues@campus.fct.unl.pt>
</commit_message>
<xml_diff>
--- a/project/Phase1/Sprint1/Burndown Chart.xlsx
+++ b/project/Phase1/Sprint1/Burndown Chart.xlsx
@@ -639,8 +639,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="2028821205"/>
-        <c:axId val="2076403543"/>
+        <c:axId val="131750862"/>
+        <c:axId val="367423202"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -714,11 +714,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2028821205"/>
-        <c:axId val="2076403543"/>
+        <c:axId val="131750862"/>
+        <c:axId val="367423202"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2028821205"/>
+        <c:axId val="131750862"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,10 +770,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2076403543"/>
+        <c:crossAx val="367423202"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2076403543"/>
+        <c:axId val="367423202"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30.0"/>
@@ -838,7 +838,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028821205"/>
+        <c:crossAx val="131750862"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1261,8 +1261,12 @@
       <c r="M6" s="16">
         <v>4.0</v>
       </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
+      <c r="N6" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="O6" s="16">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" s="17">
@@ -1301,8 +1305,12 @@
       <c r="M7" s="21">
         <v>0.0</v>
       </c>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
+      <c r="N7" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="O7" s="21">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="22" t="s">
@@ -1350,11 +1358,11 @@
       </c>
       <c r="N8" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O8" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P8" s="26"/>
     </row>
@@ -1405,11 +1413,11 @@
       </c>
       <c r="N9" s="31">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="O9" s="32">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
week1 Final day - updated charts;
Signed-off-by: GoncaloRodri <gg.rodrigues@campus.fct.unl.pt>
</commit_message>
<xml_diff>
--- a/project/Phase1/Sprint1/Burndown Chart.xlsx
+++ b/project/Phase1/Sprint1/Burndown Chart.xlsx
@@ -639,8 +639,8 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="390056067"/>
-        <c:axId val="1353689551"/>
+        <c:axId val="1541321316"/>
+        <c:axId val="1429417144"/>
       </c:barChart>
       <c:lineChart>
         <c:ser>
@@ -714,11 +714,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="390056067"/>
-        <c:axId val="1353689551"/>
+        <c:axId val="1541321316"/>
+        <c:axId val="1429417144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="390056067"/>
+        <c:axId val="1541321316"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -770,10 +770,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1353689551"/>
+        <c:crossAx val="1429417144"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1353689551"/>
+        <c:axId val="1429417144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="30.0"/>
@@ -838,7 +838,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="390056067"/>
+        <c:crossAx val="1541321316"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1265,7 +1265,7 @@
         <v>2.0</v>
       </c>
       <c r="O6" s="16">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="7">
@@ -1309,7 +1309,7 @@
         <v>1.0</v>
       </c>
       <c r="O7" s="21">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="8">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="O8" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P8" s="26"/>
     </row>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="O9" s="32">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">

</xml_diff>